<commit_message>
2 linhas a mais?
</commit_message>
<xml_diff>
--- a/AED_CP23_Saúde_Copia.xlsx
+++ b/AED_CP23_Saúde_Copia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Projeto_AED_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B18844-F021-4D71-B0D4-78B61C97C8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFE8A4-65F3-44C5-B43B-A81DEA593C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="60">
   <si>
     <t>Entidade</t>
   </si>
@@ -210,70 +210,19 @@
     <t>Questões:</t>
   </si>
   <si>
-    <t>Existe alguma relação entre as horas de sono e a média das respostas à depressão</t>
-  </si>
-  <si>
-    <t>Relação média das respostas por género (gráfico de 2 barras por género, por idade)</t>
-  </si>
-  <si>
-    <t>Definir classes de idades e analisar níveis de ansiedade por género</t>
-  </si>
-  <si>
-    <t>Como é que a saúde psicológica e o bem-estar dos alunos variam consoante o ciclo de escolaridade?</t>
-  </si>
-  <si>
     <t>O género tem impacto nas respostas relacionadas com saúde psicológica e bem-estar? Há diferenças significativas nas respostas de rapazes e raparigas?</t>
   </si>
   <si>
-    <t>Como a idade dos alunos afeta as respostas sobre saúde psicológica? Existe uma tendência de aumento ou diminuição dos problemas de saúde mental à medida que os alunos crescem?</t>
+    <t>"Existe uma correlação entre o número de horas de sono e os sintomas de depressão, ansiedade ou stress? O sono parece afetar o bem-estar psicológico de forma significativa?"</t>
   </si>
   <si>
-    <t>Existe uma correlação entre o número de horas de sono e as respostas relacionadas com sintomas de depressão, ansiedade ou stress? O sono parece afetar o bem-estar psicológico de forma significativa?</t>
+    <t>"Como os níveis de ansiedade variam por género e idade? Qual é a média das respostas relacionadas com saúde psicológica por género e idade?"</t>
   </si>
   <si>
-    <r>
-      <t>Correlação entre níveis de depressão e preocupações (v76)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
+    <t>"Existe uma relação entre a preocupação (v76) e os níveis de depressão?"</t>
   </si>
   <si>
-    <r>
-      <t>Pergunta</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: "Existe uma relação entre a preocupação (v76) e os níveis de depressão?"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Exploração</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: A variável "v76" mede o grau de preocupação. Verificar se os alunos que se preocupam mais (respostas mais altas em "v76") têm também respostas mais altas nas variáveis de depressão (v39 a v57).</t>
-    </r>
+    <t>"Como a percepção de não ter um futuro (v46) afeta a saúde psicológica dos alunos? Há uma maior prevalência de sintomas depressivos entre os alunos que sentem que não têm nada a esperar do futuro?"</t>
   </si>
 </sst>
 </file>
@@ -503,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -541,13 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -41252,10 +41194,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66113A2D-E822-48F4-BF04-52760E0C20DD}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G9" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41451,7 +41393,7 @@
       </c>
       <c r="F13" s="23"/>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -41463,7 +41405,7 @@
       </c>
       <c r="F14" s="23"/>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -41500,29 +41442,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="22"/>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="F17" s="23"/>
-      <c r="J17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="22"/>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="F18" s="23"/>
-      <c r="J18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19">
@@ -41530,7 +41466,7 @@
       </c>
       <c r="F19" s="23"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13">
@@ -41542,7 +41478,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>41</v>
       </c>
@@ -41553,27 +41489,6 @@
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J22" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J23" s="29"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J24" s="30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J25" s="29"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J26" s="30" t="s">
-        <v>64</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>